<commit_message>
Beneficiaries Update and DB Update
</commit_message>
<xml_diff>
--- a/public/storage/imports/DatabaseSeeder.xlsx
+++ b/public/storage/imports/DatabaseSeeder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dayong\public\storage\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4196FE28-2B6F-458E-8CA7-4A06B24D9297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6183023C-7785-42A3-B2A7-9700A9C20DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{72A88DDE-8111-4A1E-B739-F2F4CA7FD119}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{72A88DDE-8111-4A1E-B739-F2F4CA7FD119}"/>
   </bookViews>
   <sheets>
     <sheet name="Usertypes" sheetId="5" r:id="rId1"/>
@@ -1396,7 +1396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62750E08-8230-4924-95E5-39A7F17EECD6}">
   <dimension ref="B1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2268,9 +2268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCD2B10-2BD3-4DBC-B659-7BE7D4617E5F}">
   <dimension ref="B1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>